<commit_message>
lit searches for all proteins
</commit_message>
<xml_diff>
--- a/output/12-functional-enrichment/manual-annotations/all-BP-EnrichedGO-DML-ManAnn.xlsx
+++ b/output/12-functional-enrichment/manual-annotations/all-BP-EnrichedGO-DML-ManAnn.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yaaminivenkataraman/Documents/project-gigas-oa-meth/output/12-functional-enrichment/manual-annotations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{00A31660-6B4E-8D41-94D8-0188600F3DA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{88409110-A184-9247-B594-5C6EE0D3D833}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28800" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="1"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1719" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1728" uniqueCount="164">
   <si>
     <t>GOID</t>
   </si>
@@ -467,9 +467,6 @@
     <t>Dheilly et al. 2012 S3: Genes differentially expressed between whole stage 3 female gonads and stripped stage 3 oocytes</t>
   </si>
   <si>
-    <t>Cluster 5: Increased expression over the course of spermatogenesis (dynein ligiht chan 1, axonemal, 33 kDA inner dynein arm light chain, dynein heavy chain 3, axonemal, dynein light chan LC6, dynein heavy chain 8, dynein alpha chain, flagellar outer arm). Also highly expressed in gills and labial palps, suggesting functional similarities related to flagella and cilia structure and movement (dynein ligiht chan 1, axonemal, 33 kDA inner dynein arm light chain, dynein heavy chain 3, axonemal, dynein light chan LC6).</t>
-  </si>
-  <si>
     <t>Cluster 1: Decreased expression during gametogenesis, with higher expression in immature gonads. Also enriched for expression/high expression in adductor tissue (myosin heavy chain, striated muscle, tropomyosin), and visceral mass (myosin regulatory light chain, striated adductor muscle). Clusgter 5: Increased expression during gametogenesis (paramyosin)</t>
   </si>
   <si>
@@ -489,13 +486,370 @@
   </si>
   <si>
     <t>Serine/threonine-protein kinase Nek1: highly expressed in females over males during sex determination/differentiation</t>
+  </si>
+  <si>
+    <t>Other Notes</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Silliman 2019: Outlier SNP loci in </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>O. lurida</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, related to immune or stress response</t>
+    </r>
+  </si>
+  <si>
+    <t>Pauletto: serine/threonine kinase genes related to oocyte maturation in king scallop. Epelboin: Multiple serine/threonine-protein kinases found in eggs and embryos, including 36. Various gene expression changes in response to abiotic stressors.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Zazueta-Novoa 2014: Low accumulation and spread broadly in </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Strongylocentrotus purpuratus </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">egg and embryo during early cleavage divisions, with only a slight increase after gastrulation, relationship to ubiquitination machinery. Jiang 2011: Neuralized-like protein 2 are induced in alveolar type II cells by inflammation, control β-catenin degradation during muscle development and negatively regulate p53, which mediates apoptosis, cell growth and differentiation through the Notch signaling pathway. Up-regulation of neuralized-like protein 2 during diapause they may suppress cell division and macromolecular synthesis in </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Artemia sinica. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Hu 2005:</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Neuralized-like protein 2 may affect cell processes other than via Notch, with outcomes determined by ubiquinitation extent and the ubiquitin lysine used for attachment to target proteins</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Evans 2017: Higher expression in </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>S. purpuratus</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> populations more exposed to low pH conditions after one day of low pH exposure (embryos), but lower expression after seven days of low pH exposure (larvae). Kingtong 2013: Upregulated, energy production during spermatogenesis in </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>C. gigas.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Boonmee 2016: Associated with energy metabolism, modification of energy production during </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Pecten maximus</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> gametogenesis. Moreira 2018: Higher protein abundance when </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>C. gigas</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> exposed to As over low pH, less energy flowing through TCA cycle in low pH. Black 1962: Localized in </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>C. virginica</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> eggs and trocophores, enzyme activity increases over the course of development</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Moreira 2018: Higher in low pH + As </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>C. gigas</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, cellular stress response. Epelboin 2016: Mobilized under embryonic development and environmental stress, role in cell-cycle progression. Yao 2021: Involved in female gamete generation and oocyte development in </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Sinonovacula constricta</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (razor clam)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Leprêtre 2020: Positively regulated when exposed to contaminants, potential involvement in </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D. polymorpha</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> immunity. Zhang 2018: Upregulated in </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Marsupenaeus japonicus</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> shrimp exposed to bacteria, promotes epxression of antimicrobial peptides</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">De Witt: dynein highly expressed with relation to moving materials for calcification. Maynard 2018: Axonemal dynein is found in </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">O. lurida </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">cilia, bends microtubule complexes to generate fluid flow. Timmins-Schiffman: Differential dynein abundance in response to low pH. Goncalves 2017: Lower abundance in wild type oysters exposed to low pH. Campos 2016: Low salinity decreased dynein heavy chain 5 abundance in </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>M. edulis</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. Axonemal dyneins are associated with the microtubules movement in ciia, the cytoplasmic homolgues are primarily involved in organelle transport and centrosome assembly. Porter 1988 and Pratt 1980: Can have dynein in unfertilized sea urchin eggs</t>
+    </r>
+  </si>
+  <si>
+    <t>Cluster 5: Increased expression over the course of spermatogenesis (dynein ligiht chan 1, axonemal, 33 kDA inner dynein arm light chain, dynein heavy chain 3, axonemal, dynein light chan LC6, dynein heavy chain 8, dynein alpha chain, flagellar outer arm). Also highly expressed in gills and labial palps, suggesting functional similarities related to flagella and cilia structure and movement (dynein light chan 1, axonemal, 33 kDA inner dynein arm light chain, dynein heavy chain 3, axonemal, dynein light chan LC6).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sirotkin 2000: Unconventional myosins important for fertilization and post-fertilization embryonic processes (blastulation, gastrulation), developmentally regulated, dynamic early embryogenesis may require the activity of specific classes of myosin motor proteins. </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -635,6 +989,14 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="33">
@@ -978,13 +1340,16 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1342,8 +1707,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M183"/>
   <sheetViews>
-    <sheetView topLeftCell="A138" workbookViewId="0">
-      <selection activeCell="L124" sqref="L124"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8877,28 +9242,29 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J21"/>
+  <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="101" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="62.1640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="56.1640625" style="3" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="44.5" style="3" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="54.6640625" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="51" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="44.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="56.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44.5" style="3" customWidth="1"/>
+    <col min="4" max="4" width="54.6640625" customWidth="1"/>
+    <col min="5" max="5" width="50.83203125" customWidth="1"/>
     <col min="6" max="6" width="51" customWidth="1"/>
-    <col min="7" max="7" width="45" style="3" customWidth="1"/>
-    <col min="8" max="8" width="36.6640625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="20" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="35.83203125" style="3" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="22" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="33.33203125" style="3" customWidth="1"/>
-    <col min="11" max="16384" width="10.83203125" style="3"/>
+    <col min="10" max="10" width="33" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="61.6640625" style="3" customWidth="1"/>
+    <col min="12" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" ht="51" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>119</v>
       </c>
@@ -8915,7 +9281,7 @@
         <v>146</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>121</v>
@@ -8929,8 +9295,11 @@
       <c r="J1" s="2" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" ht="153" x14ac:dyDescent="0.2">
+      <c r="K1" s="2" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="187" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>126</v>
       </c>
@@ -8941,7 +9310,7 @@
         <v>114</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>147</v>
+        <v>162</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>114</v>
@@ -8961,8 +9330,11 @@
       <c r="J2" s="1" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" ht="119" x14ac:dyDescent="0.2">
+      <c r="K2" s="4" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="119" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>127</v>
       </c>
@@ -8973,13 +9345,13 @@
         <v>114</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>114</v>
@@ -8993,8 +9365,11 @@
       <c r="J3" s="1" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" ht="187" x14ac:dyDescent="0.2">
+      <c r="K3" s="4" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="187" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>128</v>
       </c>
@@ -9005,13 +9380,13 @@
         <v>114</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>114</v>
@@ -9025,8 +9400,11 @@
       <c r="J4" s="1" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" ht="102" x14ac:dyDescent="0.2">
+      <c r="K4" s="1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="102" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>129</v>
       </c>
@@ -9057,8 +9435,11 @@
       <c r="J5" s="1" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" ht="136" x14ac:dyDescent="0.2">
+      <c r="K5" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="221" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>130</v>
       </c>
@@ -9089,8 +9470,11 @@
       <c r="J6" s="1" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" ht="85" x14ac:dyDescent="0.2">
+      <c r="K6" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="170" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>131</v>
       </c>
@@ -9121,8 +9505,11 @@
       <c r="J7" s="1" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" ht="136" x14ac:dyDescent="0.2">
+      <c r="K7" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="136" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>132</v>
       </c>
@@ -9153,8 +9540,11 @@
       <c r="J8" s="1" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" ht="119" x14ac:dyDescent="0.2">
+      <c r="K8" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="119" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>133</v>
       </c>
@@ -9185,8 +9575,11 @@
       <c r="J9" s="1" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="K9" s="1" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>134</v>
       </c>

</xml_diff>

<commit_message>
add genes from venkataraman 2020 list
</commit_message>
<xml_diff>
--- a/output/12-functional-enrichment/manual-annotations/all-BP-EnrichedGO-DML-ManAnn.xlsx
+++ b/output/12-functional-enrichment/manual-annotations/all-BP-EnrichedGO-DML-ManAnn.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yaaminivenkataraman/Documents/project-gigas-oa-meth/output/12-functional-enrichment/manual-annotations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{88409110-A184-9247-B594-5C6EE0D3D833}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E844183-C19B-AB4A-BA62-F2126D592121}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="1"/>
+    <workbookView xWindow="28800" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="all-BP-EnrichedGO-DML-ManAnn" sheetId="1" r:id="rId1"/>
@@ -372,9 +372,6 @@
   </si>
   <si>
     <t>Venkataraman et al. 2020</t>
-  </si>
-  <si>
-    <t>dynein heavy chain 1</t>
   </si>
   <si>
     <t>unconventional myosin-XVIIIa-like</t>
@@ -844,11 +841,14 @@
   <si>
     <t xml:space="preserve">Sirotkin 2000: Unconventional myosins important for fertilization and post-fertilization embryonic processes (blastulation, gastrulation), developmentally regulated, dynamic early embryogenesis may require the activity of specific classes of myosin motor proteins. </t>
   </si>
+  <si>
+    <t>dynein heavy chain 1, 8, 12, cytoplasmic dynein 1 heavy chain 1-like, dynein heavy chain 1, cytoplasmic dynein 2 heavy chain 1-like</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1704,7 +1704,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M183"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -9241,11 +9241,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="101" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="101" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9266,51 +9266,51 @@
   <sheetData>
     <row r="1" spans="1:11" ht="51" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>146</v>
-      </c>
       <c r="F1" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>115</v>
       </c>
       <c r="I1" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="J1" s="2" t="s">
-        <v>123</v>
-      </c>
       <c r="K1" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="187" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>114</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>114</v>
@@ -9322,94 +9322,94 @@
         <v>114</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>116</v>
+        <v>163</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>114</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="119" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>114</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>114</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>114</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="187" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>114</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>114</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I4" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="J4" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="J4" s="1" t="s">
-        <v>125</v>
-      </c>
       <c r="K4" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="102" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>114</v>
@@ -9430,21 +9430,21 @@
         <v>114</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="J5" s="1" t="s">
         <v>114</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="221" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>114</v>
@@ -9465,21 +9465,21 @@
         <v>114</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="J6" s="1" t="s">
         <v>114</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="170" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>114</v>
@@ -9500,21 +9500,21 @@
         <v>114</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="J7" s="1" t="s">
         <v>114</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="136" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>114</v>
@@ -9532,24 +9532,24 @@
         <v>114</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="J8" s="1" t="s">
         <v>114</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="119" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>114</v>
@@ -9570,18 +9570,18 @@
         <v>114</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="J9" s="1" t="s">
         <v>114</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>114</v>
@@ -9605,7 +9605,7 @@
         <v>114</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="J10" s="1" t="s">
         <v>114</v>

</xml_diff>